<commit_message>
Error in files: decimal point replaced by ,
</commit_message>
<xml_diff>
--- a/pkg/vignettes/series.xlsx
+++ b/pkg/vignettes/series.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>names</t>
   </si>
@@ -55,52 +55,7 @@
     <t>C__WN___</t>
   </si>
   <si>
-    <t>6.83</t>
-  </si>
-  <si>
-    <t>6.8</t>
-  </si>
-  <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>6.71</t>
-  </si>
-  <si>
-    <t>23.34</t>
-  </si>
-  <si>
-    <t>23.24</t>
-  </si>
-  <si>
-    <t>23.20</t>
-  </si>
-  <si>
-    <t>23.68</t>
-  </si>
-  <si>
-    <t>19.35</t>
-  </si>
-  <si>
-    <t>19.38</t>
-  </si>
-  <si>
-    <t>19.58</t>
-  </si>
-  <si>
-    <t>19.68</t>
-  </si>
-  <si>
-    <t>3.84</t>
-  </si>
-  <si>
-    <t>3.54</t>
-  </si>
-  <si>
-    <t>3.74</t>
-  </si>
-  <si>
-    <t>19.69</t>
   </si>
 </sst>
 </file>
@@ -445,7 +400,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,17 +451,17 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="1">
+        <v>6.83</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>16</v>
+      <c r="F4" s="1">
+        <v>6.71</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -516,71 +471,72 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>20</v>
+      <c r="C5" s="1">
+        <v>23.34</v>
+      </c>
+      <c r="D5" s="1">
+        <v>23.34</v>
+      </c>
+      <c r="E5" s="1">
+        <v>23.2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>23.68</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>24</v>
+      <c r="C6" s="1">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="D6" s="1">
+        <v>19.38</v>
+      </c>
+      <c r="E6" s="1">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="F6" s="1">
+        <v>19.68</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>27</v>
+      <c r="C7" s="1">
+        <v>3.84</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3.84</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3.54</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3.74</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>28</v>
+      <c r="C8" s="1">
+        <v>19.38</v>
+      </c>
+      <c r="D8" s="1">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="E8" s="1">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="F8" s="1">
+        <v>19.690000000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated vignette sections: introduction, reading/writing excel files, labels, differences and period. Added section period vectors. Description lag_ts/lead_ts updated.
</commit_message>
<xml_diff>
--- a/pkg/vignettes/series.xlsx
+++ b/pkg/vignettes/series.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>names</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -91,10 +94,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -399,19 +408,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="2" max="2" width="8" style="2" customWidth="1"/>
     <col min="3" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1"/>
@@ -428,7 +435,7 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -448,8 +455,8 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="1">
         <v>6.83</v>
@@ -468,7 +475,7 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1">
@@ -504,6 +511,9 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C7" s="1">
         <v>3.84</v>

</xml_diff>

<commit_message>
Minor issues in functions lag_ts and seq.period repaired; Vignette, updated sections: introduction, reading and writing timeseries, labels, differences between multivariate ts, period and period_range, conversion between regts and df. Added a section for lags/leads/differences.
</commit_message>
<xml_diff>
--- a/pkg/vignettes/series.xlsx
+++ b/pkg/vignettes/series.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>names</t>
   </si>
   <si>
-    <t>code</t>
-  </si>
-  <si>
     <t>2017Q1</t>
   </si>
   <si>
@@ -34,9 +31,6 @@
     <t>2017Q4</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Tabel</t>
   </si>
   <si>
@@ -56,9 +50,6 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -94,16 +85,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,36 +391,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="8" style="2" customWidth="1"/>
-    <col min="3" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -447,101 +433,95 @@
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6.83</v>
       </c>
       <c r="C4" s="1">
-        <v>6.83</v>
-      </c>
-      <c r="D4" s="1">
         <v>6.8</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1">
         <v>6.71</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>23.34</v>
       </c>
       <c r="C5" s="1">
         <v>23.34</v>
       </c>
       <c r="D5" s="1">
-        <v>23.34</v>
+        <v>23.2</v>
       </c>
       <c r="E5" s="1">
-        <v>23.2</v>
-      </c>
-      <c r="F5" s="1">
         <v>23.68</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="C7" s="1">
+        <v>19.38</v>
+      </c>
+      <c r="D7" s="1">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="E7" s="1">
+        <v>19.68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3.84</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3.84</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3.54</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3.74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1">
+      <c r="B9" s="1">
+        <v>19.38</v>
+      </c>
+      <c r="C9" s="1">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="D9" s="1">
         <v>19.350000000000001</v>
       </c>
-      <c r="D6" s="1">
-        <v>19.38</v>
-      </c>
-      <c r="E6" s="1">
-        <v>19.579999999999998</v>
-      </c>
-      <c r="F6" s="1">
-        <v>19.68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3.84</v>
-      </c>
-      <c r="D7" s="1">
-        <v>3.84</v>
-      </c>
-      <c r="E7" s="1">
-        <v>3.54</v>
-      </c>
-      <c r="F7" s="1">
-        <v>3.74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1">
-        <v>19.38</v>
-      </c>
-      <c r="D8" s="1">
-        <v>19.579999999999998</v>
-      </c>
-      <c r="E8" s="1">
-        <v>19.350000000000001</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="E9" s="1">
         <v>19.690000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
NA removed in xlsx file. Generated a warning
</commit_message>
<xml_diff>
--- a/pkg/vignettes/series.xlsx
+++ b/pkg/vignettes/series.xlsx
@@ -49,7 +49,7 @@
     <t>C__WN___</t>
   </si>
   <si>
-    <t>NA</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>